<commit_message>
GrimWorld 40,000 - Core Imperialis - 3018671708 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/GrimWorld 40,000 - Core Imperialis - 3018671708/GrimWorld 40,000 - Core Imperialis - 3018671708.xlsx
+++ b/Data/GrimWorld 40,000 - Core Imperialis - 3018671708/GrimWorld 40,000 - Core Imperialis - 3018671708.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Data\haha\game\림월드 모드 번역\extractor 1.4\GrimWorld 40,000 - Core Imperialis - 3018671708\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\GrimWorld 40,000 - Core Imperialis - 3018671708\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C22FF1-A8D1-4025-858F-E0F755D6D333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47D716D-525C-4101-A583-A5559FAE5BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="1489">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -4197,6 +4197,314 @@
   </si>
   <si>
     <t>탐색</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_CarryToJob 'Carry to indoctrinating chamber' (English file: IndoctrinationChamber_Messages.xml:4)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Finished 'Conversion finished!' (English file: IndoctrinationChamber_Messages.xml:5)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Progress 'Progress' (English file: IndoctrinationChamber_Messages.xml:6)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Empty 'Waiting for loyal pawn.' (English file: IndoctrinationChamber_Messages.xml:7)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Ready 'has been converted successfully.' (English file: IndoctrinationChamber_Messages.xml:8)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_ColonistsCantUse 'Colonists can't use the chamber.' (English file: IndoctrinationChamber_Messages.xml:9)</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage 'has received brain damage from using the chamber!' (English file: IndoctrinationChamber_Messages.xml:10)</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.label 'brainwash damage'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.description 'Brainwash Damage.'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.comps.HediffComp_GetsPermanent.permanentLabel 'brainwashed'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.injuryProps.destroyedLabel 'Torn off'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.injuryProps.destroyedOutLabel 'Torn out'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.labelNoun 'brainwash damage'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamber_BrainDamage.labelNounPretty '{0} in the {1}'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamberSickness.label 'indoctrination chamber sickness'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamberSickness.description 'placeholder.'</t>
+  </si>
+  <si>
+    <t>HediffDef: IndoctrinationChamberSickness.descriptionShort 'After-effects of using a cryptosleep pod including dizziness, nausea, and vomiting.'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: indoctrination_chamber.description 'Allows for the construction of a Indoctrination chamber. Chamber allow you to recruit "unwavering loyal" pawns with risk of pernament brain damage.'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: GW_AdvancedGrimworldMaterials.label 'advanced grimworld materials'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: GW_AdvancedGrimworldMaterials.description 'Allows for the creation of advanced materials, like relic components.'</t>
+  </si>
+  <si>
+    <t>ThingDef: IndoctrinationChamber.description 'A self-powered sarcophagus designed to keep a person in a state of suspended animation for many years.'</t>
+  </si>
+  <si>
+    <t>ThingDef: GW_VehicleToolCabinet.label 'Imperial vehicle tool cabinet'</t>
+  </si>
+  <si>
+    <t>ThingDef: GW_VehicleToolCabinet.description 'Simple utility tool cabinet to speed up work around.'</t>
+  </si>
+  <si>
+    <t>ThingDef: HP_Bullet_HeavyBolter.label 'bolter round'</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef: indoctrination_chamber.label 'Indoctrination chamber'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef: IndoctrinationChamber.label 'indoctrination chamber'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_CarryToJob</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Finished</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Progress</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Empty</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_Ready</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_ColonistsCantUse</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage</t>
+  </si>
+  <si>
+    <t>Carry to indoctrinating chamber</t>
+  </si>
+  <si>
+    <t>Conversion finished!</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Waiting for loyal pawn.</t>
+  </si>
+  <si>
+    <t>has been converted successfully.</t>
+  </si>
+  <si>
+    <t>Colonists can</t>
+  </si>
+  <si>
+    <t>has received brain damage from using the chamber!</t>
+  </si>
+  <si>
+    <t>{0} in the {1}</t>
+  </si>
+  <si>
+    <t>brainwash damage</t>
+  </si>
+  <si>
+    <t>Brainwash Damage.</t>
+  </si>
+  <si>
+    <t>brainwashed</t>
+  </si>
+  <si>
+    <t>Torn off</t>
+  </si>
+  <si>
+    <t>Torn out</t>
+  </si>
+  <si>
+    <t>indoctrination chamber sickness</t>
+  </si>
+  <si>
+    <t>placeholder.</t>
+  </si>
+  <si>
+    <t>After-effects of using a cryptosleep pod including dizziness, nausea, and vomiting.</t>
+  </si>
+  <si>
+    <t>Indoctrination chamber</t>
+  </si>
+  <si>
+    <t>Allows for the construction of a Indoctrination chamber. Chamber allow you to recruit "unwavering loyal" pawns with risk of pernament brain damage.</t>
+  </si>
+  <si>
+    <t>advanced grimworld materials</t>
+  </si>
+  <si>
+    <t>Allows for the creation of advanced materials, like relic components.</t>
+  </si>
+  <si>
+    <t>indoctrination chamber</t>
+  </si>
+  <si>
+    <t>A self-powered sarcophagus designed to keep a person in a state of suspended animation for many years.</t>
+  </si>
+  <si>
+    <t>Imperial vehicle tool cabinet</t>
+  </si>
+  <si>
+    <t>Simple utility tool cabinet to speed up work around.</t>
+  </si>
+  <si>
+    <t>bolter round</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.label</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.description</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.comps.HediffComp_GetsPermanent.permanentLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.injuryProps.destroyedLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.injuryProps.destroyedOutLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.labelNoun</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.labelNounPretty</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.label</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.description</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.descriptionShort</t>
+  </si>
+  <si>
+    <t>indoctrination_chamber.label</t>
+  </si>
+  <si>
+    <t>indoctrination_chamber.description</t>
+  </si>
+  <si>
+    <t>GW_AdvancedGrimworldMaterials.label</t>
+  </si>
+  <si>
+    <t>GW_AdvancedGrimworldMaterials.description</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber.label</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber.description</t>
+  </si>
+  <si>
+    <t>GW_VehicleToolCabinet.label</t>
+  </si>
+  <si>
+    <t>GW_VehicleToolCabinet.description</t>
+  </si>
+  <si>
+    <t>HP_Bullet_HeavyBolter.label</t>
+  </si>
+  <si>
+    <t>세뇌실로 운반하기</t>
+  </si>
+  <si>
+    <t>전환 완료!</t>
+  </si>
+  <si>
+    <t>충성스러운 폰을 기다리는 중.</t>
+  </si>
+  <si>
+    <t>(이)가 성공적으로 변환되었습니다.</t>
+  </si>
+  <si>
+    <t>정착민 가능</t>
+  </si>
+  <si>
+    <t>세뇌실 사용으로 뇌 손상을 입었습니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세뇌 손상</t>
+  </si>
+  <si>
+    <t>세뇌됨</t>
+  </si>
+  <si>
+    <t>찢어짐</t>
+  </si>
+  <si>
+    <t>{1}에서 {0}</t>
+  </si>
+  <si>
+    <t>세뇌실병</t>
+  </si>
+  <si>
+    <t>(임시)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어지러움, 메스꺼움, 구토 등 동면관 사용 후유증이 발생할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>세뇌실</t>
+  </si>
+  <si>
+    <t>세뇌실을 건설할 수 있습니다. 세뇌실에서는 영구적 뇌 손상 위험이 있는 "흔들리지 않는 충성스러운" 폰을 모집할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>고급 그림월드 재료</t>
+  </si>
+  <si>
+    <t>유물 부품와 같은 고급 재료를 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>자가 동력 석관은 사람을 오랫동안 정지된 상태로 유지하도록 설계된 석관입니다.</t>
+  </si>
+  <si>
+    <t>제국 차량 공구 캐비닛</t>
+  </si>
+  <si>
+    <t>간단한 유틸리티 도구 캐비닛으로 작업 속도를 높일 수 있습니다.</t>
+  </si>
+  <si>
+    <t>볼터 탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarryToIndoctrinatingChamberJob.reportString</t>
+  </si>
+  <si>
+    <t>carrying TargetA to indoctrinating chamber.</t>
+  </si>
+  <si>
+    <t>TargetA(을)를 세뇌실로 운반 중.</t>
   </si>
 </sst>
 </file>
@@ -4570,17 +4878,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F477"/>
+  <dimension ref="A1:G504"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
+      <selection activeCell="E504" sqref="E504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
-    <col min="3" max="3" width="35.25" customWidth="1"/>
+    <col min="3" max="3" width="48.625" customWidth="1"/>
     <col min="4" max="4" width="53.75" customWidth="1"/>
     <col min="5" max="5" width="27.25" customWidth="1"/>
   </cols>
@@ -11498,7 +11806,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A465" s="5" t="s">
         <v>255</v>
       </c>
@@ -11512,7 +11820,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A466" s="5" t="s">
         <v>257</v>
       </c>
@@ -11526,7 +11834,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A467" s="5" t="s">
         <v>852</v>
       </c>
@@ -11540,7 +11848,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A468" s="5" t="s">
         <v>853</v>
       </c>
@@ -11554,7 +11862,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A469" s="5" t="s">
         <v>854</v>
       </c>
@@ -11568,7 +11876,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A470" s="5" t="s">
         <v>855</v>
       </c>
@@ -11582,7 +11890,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A471" s="5" t="s">
         <v>123</v>
       </c>
@@ -11596,7 +11904,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A472" s="5" t="s">
         <v>126</v>
       </c>
@@ -11610,7 +11918,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A473" s="5" t="s">
         <v>131</v>
       </c>
@@ -11624,7 +11932,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A474" s="5" t="s">
         <v>129</v>
       </c>
@@ -11638,7 +11946,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A475" s="5" t="s">
         <v>133</v>
       </c>
@@ -11652,7 +11960,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A476" s="5" t="s">
         <v>137</v>
       </c>
@@ -11666,7 +11974,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A477" s="5" t="s">
         <v>135</v>
       </c>
@@ -11678,6 +11986,566 @@
       </c>
       <c r="E477" s="5" t="s">
         <v>1387</v>
+      </c>
+    </row>
+    <row r="478" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B478" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C478" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D478" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E478" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F478" t="s">
+        <v>1388</v>
+      </c>
+      <c r="G478" t="str">
+        <f>MID(F478,FIND("'",F478)+1,FIND("'",F478,FIND("'",F478)+1)-FIND("'",F478)-1)</f>
+        <v>Carry to indoctrinating chamber</v>
+      </c>
+    </row>
+    <row r="479" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B479" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C479" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D479" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E479" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F479" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G479" t="str">
+        <f t="shared" ref="G479:G484" si="0">MID(F479,FIND("'",F479)+1,FIND("'",F479,FIND("'",F479)+1)-FIND("'",F479)-1)</f>
+        <v>Conversion finished!</v>
+      </c>
+    </row>
+    <row r="480" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B480" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C480" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D480" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E480" t="s">
+        <v>982</v>
+      </c>
+      <c r="F480" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G480" t="str">
+        <f t="shared" si="0"/>
+        <v>Progress</v>
+      </c>
+    </row>
+    <row r="481" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B481" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C481" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D481" t="s">
+        <v>1424</v>
+      </c>
+      <c r="E481" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F481" t="s">
+        <v>1391</v>
+      </c>
+      <c r="G481" t="str">
+        <f t="shared" si="0"/>
+        <v>Waiting for loyal pawn.</v>
+      </c>
+    </row>
+    <row r="482" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B482" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C482" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D482" t="s">
+        <v>1425</v>
+      </c>
+      <c r="E482" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F482" t="s">
+        <v>1392</v>
+      </c>
+      <c r="G482" t="str">
+        <f t="shared" si="0"/>
+        <v>has been converted successfully.</v>
+      </c>
+    </row>
+    <row r="483" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B483" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C483" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D483" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E483" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F483" t="s">
+        <v>1393</v>
+      </c>
+      <c r="G483" t="str">
+        <f t="shared" si="0"/>
+        <v>Colonists can</v>
+      </c>
+    </row>
+    <row r="484" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B484" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C484" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D484" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E484" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F484" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G484" t="str">
+        <f t="shared" si="0"/>
+        <v>has received brain damage from using the chamber!</v>
+      </c>
+    </row>
+    <row r="485" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B485" t="s">
+        <v>94</v>
+      </c>
+      <c r="C485" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D485" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E485" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F485" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G485" t="str">
+        <f t="shared" ref="G485:G503" si="1">MID(F485, FIND(": ", F485)+LEN(": "), FIND(" '", F485)-FIND(": ", F485)-LEN(": "))</f>
+        <v>IndoctrinationChamber_BrainDamage.label</v>
+      </c>
+    </row>
+    <row r="486" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B486" t="s">
+        <v>94</v>
+      </c>
+      <c r="C486" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D486" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E486" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F486" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G486" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.description</v>
+      </c>
+    </row>
+    <row r="487" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B487" t="s">
+        <v>94</v>
+      </c>
+      <c r="C487" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D487" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E487" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F487" t="s">
+        <v>1397</v>
+      </c>
+      <c r="G487" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.comps.HediffComp_GetsPermanent.permanentLabel</v>
+      </c>
+    </row>
+    <row r="488" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B488" t="s">
+        <v>94</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D488" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E488" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F488" t="s">
+        <v>1398</v>
+      </c>
+      <c r="G488" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.injuryProps.destroyedLabel</v>
+      </c>
+    </row>
+    <row r="489" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B489" t="s">
+        <v>94</v>
+      </c>
+      <c r="C489" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D489" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E489" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F489" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G489" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.injuryProps.destroyedOutLabel</v>
+      </c>
+    </row>
+    <row r="490" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B490" t="s">
+        <v>94</v>
+      </c>
+      <c r="C490" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D490" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E490" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F490" t="s">
+        <v>1400</v>
+      </c>
+      <c r="G490" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.labelNoun</v>
+      </c>
+    </row>
+    <row r="491" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B491" t="s">
+        <v>94</v>
+      </c>
+      <c r="C491" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D491" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E491" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F491" t="s">
+        <v>1401</v>
+      </c>
+      <c r="G491" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber_BrainDamage.labelNounPretty</v>
+      </c>
+    </row>
+    <row r="492" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B492" t="s">
+        <v>94</v>
+      </c>
+      <c r="C492" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D492" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E492" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F492" t="s">
+        <v>1402</v>
+      </c>
+      <c r="G492" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamberSickness.label</v>
+      </c>
+    </row>
+    <row r="493" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B493" t="s">
+        <v>94</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D493" t="s">
+        <v>1435</v>
+      </c>
+      <c r="E493" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F493" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G493" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamberSickness.description</v>
+      </c>
+    </row>
+    <row r="494" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B494" t="s">
+        <v>94</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D494" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E494" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F494" t="s">
+        <v>1404</v>
+      </c>
+      <c r="G494" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamberSickness.descriptionShort</v>
+      </c>
+    </row>
+    <row r="495" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B495" t="s">
+        <v>11</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D495" t="s">
+        <v>1437</v>
+      </c>
+      <c r="E495" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F495" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G495" t="str">
+        <f t="shared" si="1"/>
+        <v>indoctrination_chamber.label</v>
+      </c>
+    </row>
+    <row r="496" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B496" t="s">
+        <v>11</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D496" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E496" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F496" t="s">
+        <v>1405</v>
+      </c>
+      <c r="G496" t="str">
+        <f t="shared" si="1"/>
+        <v>indoctrination_chamber.description</v>
+      </c>
+    </row>
+    <row r="497" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B497" t="s">
+        <v>11</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D497" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E497" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F497" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G497" t="str">
+        <f t="shared" si="1"/>
+        <v>GW_AdvancedGrimworldMaterials.label</v>
+      </c>
+    </row>
+    <row r="498" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B498" t="s">
+        <v>11</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D498" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E498" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F498" t="s">
+        <v>1407</v>
+      </c>
+      <c r="G498" t="str">
+        <f t="shared" si="1"/>
+        <v>GW_AdvancedGrimworldMaterials.description</v>
+      </c>
+    </row>
+    <row r="499" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B499" t="s">
+        <v>143</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D499" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E499" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F499" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G499" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber.label</v>
+      </c>
+    </row>
+    <row r="500" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B500" t="s">
+        <v>143</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D500" t="s">
+        <v>1442</v>
+      </c>
+      <c r="E500" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F500" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G500" t="str">
+        <f t="shared" si="1"/>
+        <v>IndoctrinationChamber.description</v>
+      </c>
+    </row>
+    <row r="501" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B501" t="s">
+        <v>143</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D501" t="s">
+        <v>1443</v>
+      </c>
+      <c r="E501" t="s">
+        <v>1483</v>
+      </c>
+      <c r="F501" t="s">
+        <v>1409</v>
+      </c>
+      <c r="G501" t="str">
+        <f t="shared" si="1"/>
+        <v>GW_VehicleToolCabinet.label</v>
+      </c>
+    </row>
+    <row r="502" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B502" t="s">
+        <v>143</v>
+      </c>
+      <c r="C502" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D502" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E502" t="s">
+        <v>1484</v>
+      </c>
+      <c r="F502" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G502" t="str">
+        <f t="shared" si="1"/>
+        <v>GW_VehicleToolCabinet.description</v>
+      </c>
+    </row>
+    <row r="503" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B503" t="s">
+        <v>143</v>
+      </c>
+      <c r="C503" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D503" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E503" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F503" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G503" t="str">
+        <f t="shared" si="1"/>
+        <v>HP_Bullet_HeavyBolter.label</v>
+      </c>
+    </row>
+    <row r="504" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B504" t="s">
+        <v>119</v>
+      </c>
+      <c r="C504" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D504" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E504" t="s">
+        <v>1488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GrimWorld 40,000 - Core Imperialis 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/GrimWorld 40,000 - Core Imperialis - 3018671708/GrimWorld 40,000 - Core Imperialis - 3018671708.xlsx
+++ b/Data/GrimWorld 40,000 - Core Imperialis - 3018671708/GrimWorld 40,000 - Core Imperialis - 3018671708.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\GrimWorld 40,000 - Core Imperialis - 3018671708\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47D716D-525C-4101-A583-A5559FAE5BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DC0D49-CE6A-41B8-8C13-B4F888F05525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="1489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="1611">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -4463,9 +4463,6 @@
     <t>{1}에서 {0}</t>
   </si>
   <si>
-    <t>세뇌실병</t>
-  </si>
-  <si>
     <t>(임시)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4505,6 +4502,378 @@
   </si>
   <si>
     <t>TargetA(을)를 세뇌실로 운반 중.</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.1.name 'Black Templars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.2.name 'Blood Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.3.name 'Blood Ravens'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.4.name 'Dark Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.5.name 'Imperial Fists'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.6.name 'Iron Hands'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.7.name 'Raven Guard'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.9.name 'Space Wolves'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.11.name 'White Scars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.0.name 'Astra Revanents'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.1.name 'Black Templars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.2.name 'Blood Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.3.name 'Blood Ravens'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.4.name 'Dark Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.5.name 'Imperial Fists'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.6.name 'Iron Hands'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.7.name 'Raven Guard'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.9.name 'Space Wolves'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_HelmetChapterPalettes.palettes.11.name 'White Scars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.0.name 'Astra Revanents'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.1.name 'Black Templars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.2.name 'Blood Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.3.name 'Blood Ravens'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.4.name 'Dark Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.5.name 'Imperial Fists'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.6.name 'Iron Hands'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.7.name 'Raven Guard'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.9.name 'Space Wolves'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShoulderChapterPalettes.palettes.11.name 'White Scars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.0.name 'Astra Revanents'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.1.name 'Black Templars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.2.name 'Blood Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.3.name 'Blood Ravens'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.4.name 'Dark Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.5.name 'Imperial Fists'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.6.name 'Iron Hands'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.7.name 'Raven Guard'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.9.name 'Space Wolves'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_BackpackChapterPalettes.palettes.11.name 'White Scars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.0.name 'Astra Revanents'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.1.name 'Black Templars'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.2.name 'Blood Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.3.name 'Blood Ravens'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.4.name 'Dark Angels'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.5.name 'Imperial Fists'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.6.name 'Iron Hands'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.7.name 'Raven Guard'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.9.name 'Space Wolves'</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_ShieldChapterPalettes.palettes.11.name 'White Scars'</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.0.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.1.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.2.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.3.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.4.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.5.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.6.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.7.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.9.name</t>
+  </si>
+  <si>
+    <t>GW_SM_TorsoChapterPalettes.palettes.11.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.0.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.1.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.2.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.3.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.4.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.5.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.6.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.7.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.9.name</t>
+  </si>
+  <si>
+    <t>GW_SM_HelmetChapterPalettes.palettes.11.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.0.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.1.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.2.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.3.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.4.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.5.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.6.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.7.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.9.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShoulderChapterPalettes.palettes.11.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.0.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.1.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.2.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.3.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.4.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.5.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.6.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.7.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.9.name</t>
+  </si>
+  <si>
+    <t>GW_SM_BackpackChapterPalettes.palettes.11.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.0.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.1.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.2.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.3.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.4.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.5.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.6.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.7.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.9.name</t>
+  </si>
+  <si>
+    <t>GW_SM_ShieldChapterPalettes.palettes.11.name</t>
+  </si>
+  <si>
+    <t>PaletteDef: GW_SM_TorsoChapterPalettes.palettes.0.name 'Astra Revanents'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PaletteDef</t>
+  </si>
+  <si>
+    <t>Astra Revanents</t>
+  </si>
+  <si>
+    <t>Black Templars</t>
+  </si>
+  <si>
+    <t>Blood Angels</t>
+  </si>
+  <si>
+    <t>Blood Ravens</t>
+  </si>
+  <si>
+    <t>Dark Angels</t>
+  </si>
+  <si>
+    <t>Imperial Fists</t>
+  </si>
+  <si>
+    <t>Iron Hands</t>
+  </si>
+  <si>
+    <t>Raven Guard</t>
+  </si>
+  <si>
+    <t>Space Wolves</t>
+  </si>
+  <si>
+    <t>White Scars</t>
+  </si>
+  <si>
+    <t>Astra Revanents</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아스트라 레버넌트</t>
+  </si>
+  <si>
+    <t>블랙 템플러</t>
+  </si>
+  <si>
+    <t>블러드 엔젤</t>
+  </si>
+  <si>
+    <t>블러드 레이븐</t>
+  </si>
+  <si>
+    <t>다크 엔젤</t>
+  </si>
+  <si>
+    <t>임페리얼 피스트</t>
+  </si>
+  <si>
+    <t>아이언 핸드</t>
+  </si>
+  <si>
+    <t>레이븐 가드</t>
+  </si>
+  <si>
+    <t>스페이스 울프</t>
+  </si>
+  <si>
+    <t>세뇌실병</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화이트 스카</t>
   </si>
 </sst>
 </file>
@@ -4878,10 +5247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G504"/>
+  <dimension ref="A1:G554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
-      <selection activeCell="E504" sqref="E504"/>
+    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
+      <selection activeCell="D435" sqref="D435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12152,7 +12521,7 @@
         <v>1395</v>
       </c>
       <c r="G485" t="str">
-        <f t="shared" ref="G485:G503" si="1">MID(F485, FIND(": ", F485)+LEN(": "), FIND(" '", F485)-FIND(": ", F485)-LEN(": "))</f>
+        <f t="shared" ref="G485:G548" si="1">MID(F485, FIND(": ", F485)+LEN(": "), FIND(" '", F485)-FIND(": ", F485)-LEN(": "))</f>
         <v>IndoctrinationChamber_BrainDamage.label</v>
       </c>
     </row>
@@ -12293,7 +12662,7 @@
         <v>1434</v>
       </c>
       <c r="E492" t="s">
-        <v>1475</v>
+        <v>1609</v>
       </c>
       <c r="F492" t="s">
         <v>1402</v>
@@ -12314,7 +12683,7 @@
         <v>1435</v>
       </c>
       <c r="E493" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="F493" t="s">
         <v>1403</v>
@@ -12335,7 +12704,7 @@
         <v>1436</v>
       </c>
       <c r="E494" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="F494" t="s">
         <v>1404</v>
@@ -12356,7 +12725,7 @@
         <v>1437</v>
       </c>
       <c r="E495" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="F495" t="s">
         <v>1412</v>
@@ -12377,7 +12746,7 @@
         <v>1438</v>
       </c>
       <c r="E496" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="F496" t="s">
         <v>1405</v>
@@ -12398,7 +12767,7 @@
         <v>1439</v>
       </c>
       <c r="E497" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="F497" t="s">
         <v>1406</v>
@@ -12419,7 +12788,7 @@
         <v>1440</v>
       </c>
       <c r="E498" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="F498" t="s">
         <v>1407</v>
@@ -12440,7 +12809,7 @@
         <v>1441</v>
       </c>
       <c r="E499" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="F499" t="s">
         <v>1413</v>
@@ -12461,7 +12830,7 @@
         <v>1442</v>
       </c>
       <c r="E500" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="F500" t="s">
         <v>1408</v>
@@ -12482,7 +12851,7 @@
         <v>1443</v>
       </c>
       <c r="E501" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="F501" t="s">
         <v>1409</v>
@@ -12503,7 +12872,7 @@
         <v>1444</v>
       </c>
       <c r="E502" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="F502" t="s">
         <v>1410</v>
@@ -12524,7 +12893,7 @@
         <v>1445</v>
       </c>
       <c r="E503" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="F503" t="s">
         <v>1411</v>
@@ -12539,13 +12908,1067 @@
         <v>119</v>
       </c>
       <c r="C504" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D504" t="s">
         <v>1486</v>
       </c>
-      <c r="D504" t="s">
+      <c r="E504" t="s">
         <v>1487</v>
       </c>
-      <c r="E504" t="s">
+      <c r="G504" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="505" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B505" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C505" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D505" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E505" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F505" t="s">
+        <v>1587</v>
+      </c>
+      <c r="G505" t="str">
+        <f>MID(F505,FIND("'",F505)+1,FIND("'",F505,FIND("'",F505)+1)-FIND("'",F505)-1)</f>
+        <v>Astra Revanents</v>
+      </c>
+    </row>
+    <row r="506" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B506" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C506" t="s">
+        <v>1538</v>
+      </c>
+      <c r="D506" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E506" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F506" t="s">
         <v>1488</v>
+      </c>
+      <c r="G506" t="str">
+        <f t="shared" ref="G506:G554" si="2">MID(F506,FIND("'",F506)+1,FIND("'",F506,FIND("'",F506)+1)-FIND("'",F506)-1)</f>
+        <v>Black Templars</v>
+      </c>
+    </row>
+    <row r="507" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B507" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C507" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D507" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E507" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F507" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G507" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Angels</v>
+      </c>
+    </row>
+    <row r="508" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B508" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C508" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D508" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E508" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F508" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G508" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Ravens</v>
+      </c>
+    </row>
+    <row r="509" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B509" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C509" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D509" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E509" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F509" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G509" t="str">
+        <f t="shared" si="2"/>
+        <v>Dark Angels</v>
+      </c>
+    </row>
+    <row r="510" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B510" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C510" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D510" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E510" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F510" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G510" t="str">
+        <f t="shared" si="2"/>
+        <v>Imperial Fists</v>
+      </c>
+    </row>
+    <row r="511" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B511" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C511" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D511" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E511" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F511" t="s">
+        <v>1493</v>
+      </c>
+      <c r="G511" t="str">
+        <f t="shared" si="2"/>
+        <v>Iron Hands</v>
+      </c>
+    </row>
+    <row r="512" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B512" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C512" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D512" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E512" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F512" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G512" t="str">
+        <f t="shared" si="2"/>
+        <v>Raven Guard</v>
+      </c>
+    </row>
+    <row r="513" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B513" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D513" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E513" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F513" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G513" t="str">
+        <f t="shared" si="2"/>
+        <v>Space Wolves</v>
+      </c>
+    </row>
+    <row r="514" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B514" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C514" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D514" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E514" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F514" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G514" t="str">
+        <f t="shared" si="2"/>
+        <v>White Scars</v>
+      </c>
+    </row>
+    <row r="515" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B515" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C515" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D515" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E515" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F515" t="s">
+        <v>1497</v>
+      </c>
+      <c r="G515" t="str">
+        <f t="shared" si="2"/>
+        <v>Astra Revanents</v>
+      </c>
+    </row>
+    <row r="516" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B516" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C516" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D516" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E516" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F516" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G516" t="str">
+        <f t="shared" si="2"/>
+        <v>Black Templars</v>
+      </c>
+    </row>
+    <row r="517" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B517" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C517" t="s">
+        <v>1549</v>
+      </c>
+      <c r="D517" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E517" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F517" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G517" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Angels</v>
+      </c>
+    </row>
+    <row r="518" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B518" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C518" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D518" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E518" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F518" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G518" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Ravens</v>
+      </c>
+    </row>
+    <row r="519" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B519" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C519" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D519" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E519" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F519" t="s">
+        <v>1501</v>
+      </c>
+      <c r="G519" t="str">
+        <f t="shared" si="2"/>
+        <v>Dark Angels</v>
+      </c>
+    </row>
+    <row r="520" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B520" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C520" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D520" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E520" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F520" t="s">
+        <v>1502</v>
+      </c>
+      <c r="G520" t="str">
+        <f t="shared" si="2"/>
+        <v>Imperial Fists</v>
+      </c>
+    </row>
+    <row r="521" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B521" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C521" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D521" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E521" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F521" t="s">
+        <v>1503</v>
+      </c>
+      <c r="G521" t="str">
+        <f t="shared" si="2"/>
+        <v>Iron Hands</v>
+      </c>
+    </row>
+    <row r="522" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B522" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C522" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D522" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E522" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F522" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G522" t="str">
+        <f t="shared" si="2"/>
+        <v>Raven Guard</v>
+      </c>
+    </row>
+    <row r="523" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B523" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1555</v>
+      </c>
+      <c r="D523" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E523" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F523" t="s">
+        <v>1505</v>
+      </c>
+      <c r="G523" t="str">
+        <f t="shared" si="2"/>
+        <v>Space Wolves</v>
+      </c>
+    </row>
+    <row r="524" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B524" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C524" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D524" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E524" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F524" t="s">
+        <v>1506</v>
+      </c>
+      <c r="G524" t="str">
+        <f t="shared" si="2"/>
+        <v>White Scars</v>
+      </c>
+    </row>
+    <row r="525" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B525" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C525" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D525" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E525" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F525" t="s">
+        <v>1507</v>
+      </c>
+      <c r="G525" t="str">
+        <f t="shared" si="2"/>
+        <v>Astra Revanents</v>
+      </c>
+    </row>
+    <row r="526" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B526" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C526" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D526" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E526" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F526" t="s">
+        <v>1508</v>
+      </c>
+      <c r="G526" t="str">
+        <f t="shared" si="2"/>
+        <v>Black Templars</v>
+      </c>
+    </row>
+    <row r="527" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B527" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C527" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D527" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E527" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F527" t="s">
+        <v>1509</v>
+      </c>
+      <c r="G527" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Angels</v>
+      </c>
+    </row>
+    <row r="528" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B528" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C528" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D528" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E528" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F528" t="s">
+        <v>1510</v>
+      </c>
+      <c r="G528" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Ravens</v>
+      </c>
+    </row>
+    <row r="529" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B529" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C529" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D529" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E529" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F529" t="s">
+        <v>1511</v>
+      </c>
+      <c r="G529" t="str">
+        <f t="shared" si="2"/>
+        <v>Dark Angels</v>
+      </c>
+    </row>
+    <row r="530" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B530" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C530" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D530" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E530" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F530" t="s">
+        <v>1512</v>
+      </c>
+      <c r="G530" t="str">
+        <f t="shared" si="2"/>
+        <v>Imperial Fists</v>
+      </c>
+    </row>
+    <row r="531" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B531" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C531" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D531" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E531" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F531" t="s">
+        <v>1513</v>
+      </c>
+      <c r="G531" t="str">
+        <f t="shared" si="2"/>
+        <v>Iron Hands</v>
+      </c>
+    </row>
+    <row r="532" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B532" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C532" t="s">
+        <v>1564</v>
+      </c>
+      <c r="D532" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E532" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F532" t="s">
+        <v>1514</v>
+      </c>
+      <c r="G532" t="str">
+        <f t="shared" si="2"/>
+        <v>Raven Guard</v>
+      </c>
+    </row>
+    <row r="533" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B533" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C533" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D533" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E533" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F533" t="s">
+        <v>1515</v>
+      </c>
+      <c r="G533" t="str">
+        <f t="shared" si="2"/>
+        <v>Space Wolves</v>
+      </c>
+    </row>
+    <row r="534" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B534" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C534" t="s">
+        <v>1566</v>
+      </c>
+      <c r="D534" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E534" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F534" t="s">
+        <v>1516</v>
+      </c>
+      <c r="G534" t="str">
+        <f t="shared" si="2"/>
+        <v>White Scars</v>
+      </c>
+    </row>
+    <row r="535" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B535" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C535" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D535" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E535" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F535" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G535" t="str">
+        <f t="shared" si="2"/>
+        <v>Astra Revanents</v>
+      </c>
+    </row>
+    <row r="536" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B536" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C536" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D536" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E536" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F536" t="s">
+        <v>1518</v>
+      </c>
+      <c r="G536" t="str">
+        <f t="shared" si="2"/>
+        <v>Black Templars</v>
+      </c>
+    </row>
+    <row r="537" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B537" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C537" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D537" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E537" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F537" t="s">
+        <v>1519</v>
+      </c>
+      <c r="G537" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Angels</v>
+      </c>
+    </row>
+    <row r="538" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B538" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C538" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D538" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E538" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F538" t="s">
+        <v>1520</v>
+      </c>
+      <c r="G538" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Ravens</v>
+      </c>
+    </row>
+    <row r="539" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B539" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C539" t="s">
+        <v>1571</v>
+      </c>
+      <c r="D539" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E539" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F539" t="s">
+        <v>1521</v>
+      </c>
+      <c r="G539" t="str">
+        <f t="shared" si="2"/>
+        <v>Dark Angels</v>
+      </c>
+    </row>
+    <row r="540" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B540" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C540" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D540" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E540" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F540" t="s">
+        <v>1522</v>
+      </c>
+      <c r="G540" t="str">
+        <f t="shared" si="2"/>
+        <v>Imperial Fists</v>
+      </c>
+    </row>
+    <row r="541" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B541" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C541" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D541" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E541" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F541" t="s">
+        <v>1523</v>
+      </c>
+      <c r="G541" t="str">
+        <f t="shared" si="2"/>
+        <v>Iron Hands</v>
+      </c>
+    </row>
+    <row r="542" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B542" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C542" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D542" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E542" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F542" t="s">
+        <v>1524</v>
+      </c>
+      <c r="G542" t="str">
+        <f t="shared" si="2"/>
+        <v>Raven Guard</v>
+      </c>
+    </row>
+    <row r="543" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B543" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C543" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D543" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E543" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F543" t="s">
+        <v>1525</v>
+      </c>
+      <c r="G543" t="str">
+        <f t="shared" si="2"/>
+        <v>Space Wolves</v>
+      </c>
+    </row>
+    <row r="544" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B544" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C544" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E544" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F544" t="s">
+        <v>1526</v>
+      </c>
+      <c r="G544" t="str">
+        <f t="shared" si="2"/>
+        <v>White Scars</v>
+      </c>
+    </row>
+    <row r="545" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B545" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C545" t="s">
+        <v>1577</v>
+      </c>
+      <c r="D545" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E545" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F545" t="s">
+        <v>1527</v>
+      </c>
+      <c r="G545" t="str">
+        <f t="shared" si="2"/>
+        <v>Astra Revanents</v>
+      </c>
+    </row>
+    <row r="546" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B546" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C546" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D546" t="s">
+        <v>1590</v>
+      </c>
+      <c r="E546" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F546" t="s">
+        <v>1528</v>
+      </c>
+      <c r="G546" t="str">
+        <f t="shared" si="2"/>
+        <v>Black Templars</v>
+      </c>
+    </row>
+    <row r="547" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B547" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C547" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D547" t="s">
+        <v>1591</v>
+      </c>
+      <c r="E547" t="s">
+        <v>1602</v>
+      </c>
+      <c r="F547" t="s">
+        <v>1529</v>
+      </c>
+      <c r="G547" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Angels</v>
+      </c>
+    </row>
+    <row r="548" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B548" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C548" t="s">
+        <v>1580</v>
+      </c>
+      <c r="D548" t="s">
+        <v>1592</v>
+      </c>
+      <c r="E548" t="s">
+        <v>1603</v>
+      </c>
+      <c r="F548" t="s">
+        <v>1530</v>
+      </c>
+      <c r="G548" t="str">
+        <f t="shared" si="2"/>
+        <v>Blood Ravens</v>
+      </c>
+    </row>
+    <row r="549" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B549" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C549" t="s">
+        <v>1581</v>
+      </c>
+      <c r="D549" t="s">
+        <v>1593</v>
+      </c>
+      <c r="E549" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F549" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G549" t="str">
+        <f t="shared" si="2"/>
+        <v>Dark Angels</v>
+      </c>
+    </row>
+    <row r="550" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B550" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C550" t="s">
+        <v>1582</v>
+      </c>
+      <c r="D550" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E550" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F550" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G550" t="str">
+        <f t="shared" si="2"/>
+        <v>Imperial Fists</v>
+      </c>
+    </row>
+    <row r="551" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B551" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C551" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D551" t="s">
+        <v>1595</v>
+      </c>
+      <c r="E551" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F551" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G551" t="str">
+        <f t="shared" si="2"/>
+        <v>Iron Hands</v>
+      </c>
+    </row>
+    <row r="552" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B552" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C552" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D552" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E552" t="s">
+        <v>1607</v>
+      </c>
+      <c r="F552" t="s">
+        <v>1534</v>
+      </c>
+      <c r="G552" t="str">
+        <f t="shared" si="2"/>
+        <v>Raven Guard</v>
+      </c>
+    </row>
+    <row r="553" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B553" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C553" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D553" t="s">
+        <v>1597</v>
+      </c>
+      <c r="E553" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F553" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G553" t="str">
+        <f t="shared" si="2"/>
+        <v>Space Wolves</v>
+      </c>
+    </row>
+    <row r="554" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B554" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C554" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D554" t="s">
+        <v>1598</v>
+      </c>
+      <c r="E554" t="s">
+        <v>1610</v>
+      </c>
+      <c r="F554" t="s">
+        <v>1536</v>
+      </c>
+      <c r="G554" t="str">
+        <f t="shared" si="2"/>
+        <v>White Scars</v>
       </c>
     </row>
   </sheetData>

</xml_diff>